<commit_message>
Create and Delete Folders
</commit_message>
<xml_diff>
--- a/src/main/java/com/unifier/automation/dmautomation/data/TestData.xlsx
+++ b/src/main/java/com/unifier/automation/dmautomation/data/TestData.xlsx
@@ -414,7 +414,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,7 +453,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>